<commit_message>
STAGE 1 COMPLETE: Enhanced import summary with clearer labels and better UX
</commit_message>
<xml_diff>
--- a/portfolio_corrected_costs.xlsx
+++ b/portfolio_corrected_costs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/db67c74c26241c9d/Saudi Stock Market App/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="444" documentId="11_09498FE762541E89FE26B2F73C20F2D03CD5F7CF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EFEB9949-D62B-42F5-A70B-20293AD7FB3A}"/>
+  <xr:revisionPtr revIDLastSave="445" documentId="11_09498FE762541E89FE26B2F73C20F2D03CD5F7CF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9F6F7C4-D733-421C-87F3-0B4740934F3C}"/>
   <bookViews>
     <workbookView xWindow="-65040" yWindow="-2160" windowWidth="33450" windowHeight="15750" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6977,8 +6977,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A13" sqref="A1:XFD13"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D13" sqref="D2:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -6989,7 +6989,7 @@
     <col min="7" max="7" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" hidden="1">
+    <row r="1" spans="1:7" ht="15">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7007,7 +7007,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" hidden="1">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7031,7 +7031,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:7" hidden="1">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2</v>
       </c>
@@ -7055,7 +7055,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" hidden="1">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
@@ -7079,7 +7079,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:7" hidden="1">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>4</v>
       </c>
@@ -7103,7 +7103,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:7" hidden="1">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>5</v>
       </c>
@@ -7127,7 +7127,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" hidden="1">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>6</v>
       </c>
@@ -7151,7 +7151,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" hidden="1">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>7</v>
       </c>
@@ -7175,7 +7175,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:7" hidden="1">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>8</v>
       </c>
@@ -7199,7 +7199,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:7" hidden="1">
+    <row r="10" spans="1:7">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
         <v>38</v>
@@ -7221,7 +7221,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:7" hidden="1">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>9</v>
       </c>
@@ -7245,7 +7245,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:7" hidden="1">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>10</v>
       </c>
@@ -7269,7 +7269,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:7" hidden="1">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
🚀 Complete Modern TADAWUL NEXUS with Risk Management & Analytics
✨ Features Added:
• Complete modern portfolio management interface
• Risk Management section with comprehensive tools
• Advanced Analytics dashboard
• Professional table styling with sequential numbering
• Enhanced dropdown visibility and UI improvements
• Expandable navigation menu system
• Multiple portfolio view modes
• Comprehensive workspace cleanup

🔧 Technical Improvements:
• Fixed CSS styling for all components
• Improved data processing and display
• Enhanced user experience across all sections
• Professional branding and visual design
• Optimized performance and responsiveness
</commit_message>
<xml_diff>
--- a/portfolio_corrected_costs.xlsx
+++ b/portfolio_corrected_costs.xlsx
@@ -1,24 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/db67c74c26241c9d/Saudi Stock Market App/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="445" documentId="11_09498FE762541E89FE26B2F73C20F2D03CD5F7CF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9F6F7C4-D733-421C-87F3-0B4740934F3C}"/>
+  <xr:revisionPtr revIDLastSave="522" documentId="11_09498FE762541E89FE26B2F73C20F2D03CD5F7CF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40177C3E-8983-4511-9EA2-B4FF156679B7}"/>
   <bookViews>
-    <workbookView xWindow="-65040" yWindow="-2160" windowWidth="33450" windowHeight="15750" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-80520" yWindow="-3945" windowWidth="51840" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Orginal Stock Market STock  (2)" sheetId="5" r:id="rId1"/>
     <sheet name="Your Portfolio" sheetId="1" r:id="rId2"/>
-    <sheet name="Orginal Stock Market STock List" sheetId="4" r:id="rId3"/>
-    <sheet name="Empty Template" sheetId="2" r:id="rId4"/>
-    <sheet name="Sheet4" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId3"/>
+    <sheet name="Orginal Stock Market STock List" sheetId="4" r:id="rId4"/>
+    <sheet name="Empty Template" sheetId="2" r:id="rId5"/>
+    <sheet name="Sheet4" sheetId="6" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Your Portfolio'!$A$1:$G$41</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1868" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2168" uniqueCount="527">
   <si>
     <t>Company</t>
   </si>
@@ -940,6 +944,684 @@
   </si>
   <si>
     <t>Sector</t>
+  </si>
+  <si>
+    <t>Al Hamadi</t>
+  </si>
+  <si>
+    <t>27.76 SAR</t>
+  </si>
+  <si>
+    <t>108,582.98 SAR</t>
+  </si>
+  <si>
+    <t>-2,712.21 SAR</t>
+  </si>
+  <si>
+    <t>-2.50%</t>
+  </si>
+  <si>
+    <t>13.67 SAR</t>
+  </si>
+  <si>
+    <t>144,163.82 SAR</t>
+  </si>
+  <si>
+    <t>-11,916.98 SAR</t>
+  </si>
+  <si>
+    <t>-8.27%</t>
+  </si>
+  <si>
+    <t>21.78 SAR</t>
+  </si>
+  <si>
+    <t>79,845.48 SAR</t>
+  </si>
+  <si>
+    <t>+2,236.26 SAR</t>
+  </si>
+  <si>
+    <t>+2.80%</t>
+  </si>
+  <si>
+    <t>27.31 SAR</t>
+  </si>
+  <si>
+    <t>40,965.00 SAR</t>
+  </si>
+  <si>
+    <t>-990.00 SAR</t>
+  </si>
+  <si>
+    <t>-2.42%</t>
+  </si>
+  <si>
+    <t>27.02 SAR</t>
+  </si>
+  <si>
+    <t>100,568.44 SAR</t>
+  </si>
+  <si>
+    <t>-4,987.48 SAR</t>
+  </si>
+  <si>
+    <t>-4.96%</t>
+  </si>
+  <si>
+    <t>36.04 SAR</t>
+  </si>
+  <si>
+    <t>72,080.00 SAR</t>
+  </si>
+  <si>
+    <t>-800.00 SAR</t>
+  </si>
+  <si>
+    <t>-1.11%</t>
+  </si>
+  <si>
+    <t>38.69 SAR</t>
+  </si>
+  <si>
+    <t>38,690.00 SAR</t>
+  </si>
+  <si>
+    <t>34.97 SAR</t>
+  </si>
+  <si>
+    <t>34,970.00 SAR</t>
+  </si>
+  <si>
+    <t>-3,720.00 SAR</t>
+  </si>
+  <si>
+    <t>-9.61%</t>
+  </si>
+  <si>
+    <t>92.60 SAR</t>
+  </si>
+  <si>
+    <t>46,300.00 SAR</t>
+  </si>
+  <si>
+    <t>96.99 SAR</t>
+  </si>
+  <si>
+    <t>48,495.00 SAR</t>
+  </si>
+  <si>
+    <t>+2,195.00 SAR</t>
+  </si>
+  <si>
+    <t>+4.74%</t>
+  </si>
+  <si>
+    <t>71.97 SAR</t>
+  </si>
+  <si>
+    <t>215,910.00 SAR</t>
+  </si>
+  <si>
+    <t>-29,640.00 SAR</t>
+  </si>
+  <si>
+    <t>-13.73%</t>
+  </si>
+  <si>
+    <t>62.74 SAR</t>
+  </si>
+  <si>
+    <t>66,567.14 SAR</t>
+  </si>
+  <si>
+    <t>-41,156.19 SAR</t>
+  </si>
+  <si>
+    <t>-61.83%</t>
+  </si>
+  <si>
+    <t>10.86 SAR</t>
+  </si>
+  <si>
+    <t>59,730.00 SAR</t>
+  </si>
+  <si>
+    <t>+495.00 SAR</t>
+  </si>
+  <si>
+    <t>+0.83%</t>
+  </si>
+  <si>
+    <t>31.99 SAR</t>
+  </si>
+  <si>
+    <t>47,985.00 SAR</t>
+  </si>
+  <si>
+    <t>-7,200.00 SAR</t>
+  </si>
+  <si>
+    <t>-15.00%</t>
+  </si>
+  <si>
+    <t>34.50 SAR</t>
+  </si>
+  <si>
+    <t>34,500.00 SAR</t>
+  </si>
+  <si>
+    <t>21.41 SAR</t>
+  </si>
+  <si>
+    <t>21,410.00 SAR</t>
+  </si>
+  <si>
+    <t>-13,090.00 SAR</t>
+  </si>
+  <si>
+    <t>-37.94%</t>
+  </si>
+  <si>
+    <t>7.62 SAR</t>
+  </si>
+  <si>
+    <t>7,620.00 SAR</t>
+  </si>
+  <si>
+    <t>15.77 SAR</t>
+  </si>
+  <si>
+    <t>15,770.00 SAR</t>
+  </si>
+  <si>
+    <t>+8,150.00 SAR</t>
+  </si>
+  <si>
+    <t>+106.96%</t>
+  </si>
+  <si>
+    <t>2.00 SAR</t>
+  </si>
+  <si>
+    <t>1,292.00 SAR</t>
+  </si>
+  <si>
+    <t>+28,740.54 SAR</t>
+  </si>
+  <si>
+    <t>+2224.50%</t>
+  </si>
+  <si>
+    <t>34.34 SAR</t>
+  </si>
+  <si>
+    <t>133,136.18 SAR</t>
+  </si>
+  <si>
+    <t>34.79 SAR</t>
+  </si>
+  <si>
+    <t>134,880.83 SAR</t>
+  </si>
+  <si>
+    <t>+1,744.65 SAR</t>
+  </si>
+  <si>
+    <t>+1.31%</t>
+  </si>
+  <si>
+    <t>14.72 SAR</t>
+  </si>
+  <si>
+    <t>14,720.00 SAR</t>
+  </si>
+  <si>
+    <t>+140.00 SAR</t>
+  </si>
+  <si>
+    <t>+0.95%</t>
+  </si>
+  <si>
+    <t>62.51 SAR</t>
+  </si>
+  <si>
+    <t>60,759.72 SAR</t>
+  </si>
+  <si>
+    <t>38.17 SAR</t>
+  </si>
+  <si>
+    <t>37,101.24 SAR</t>
+  </si>
+  <si>
+    <t>-23,658.48 SAR</t>
+  </si>
+  <si>
+    <t>-38.94%</t>
+  </si>
+  <si>
+    <t>10.75 SAR</t>
+  </si>
+  <si>
+    <t>102,125.00 SAR</t>
+  </si>
+  <si>
+    <t>+199,120.00 SAR</t>
+  </si>
+  <si>
+    <t>+194.98%</t>
+  </si>
+  <si>
+    <t>25.92 SAR</t>
+  </si>
+  <si>
+    <t>259.20 SAR</t>
+  </si>
+  <si>
+    <t>28.90 SAR</t>
+  </si>
+  <si>
+    <t>289.00 SAR</t>
+  </si>
+  <si>
+    <t>+29.80 SAR</t>
+  </si>
+  <si>
+    <t>+11.50%</t>
+  </si>
+  <si>
+    <t>2.26 SAR</t>
+  </si>
+  <si>
+    <t>15,368.00 SAR</t>
+  </si>
+  <si>
+    <t>+151,504.00 SAR</t>
+  </si>
+  <si>
+    <t>+985.84%</t>
+  </si>
+  <si>
+    <t>7.79 SAR</t>
+  </si>
+  <si>
+    <t>31,160.00 SAR</t>
+  </si>
+  <si>
+    <t>+102,680.00 SAR</t>
+  </si>
+  <si>
+    <t>+329.53%</t>
+  </si>
+  <si>
+    <t>13.57 SAR</t>
+  </si>
+  <si>
+    <t>116,335.61 SAR</t>
+  </si>
+  <si>
+    <t>25.34 SAR</t>
+  </si>
+  <si>
+    <t>217,239.82 SAR</t>
+  </si>
+  <si>
+    <t>+100,904.21 SAR</t>
+  </si>
+  <si>
+    <t>+86.74%</t>
+  </si>
+  <si>
+    <t>14.43 SAR</t>
+  </si>
+  <si>
+    <t>57,720.00 SAR</t>
+  </si>
+  <si>
+    <t>28.64 SAR</t>
+  </si>
+  <si>
+    <t>114,560.00 SAR</t>
+  </si>
+  <si>
+    <t>+56,840.00 SAR</t>
+  </si>
+  <si>
+    <t>+98.48%</t>
+  </si>
+  <si>
+    <t>42.86 SAR</t>
+  </si>
+  <si>
+    <t>55,718.00 SAR</t>
+  </si>
+  <si>
+    <t>39.21 SAR</t>
+  </si>
+  <si>
+    <t>50,973.00 SAR</t>
+  </si>
+  <si>
+    <t>-4,745.00 SAR</t>
+  </si>
+  <si>
+    <t>-8.52%</t>
+  </si>
+  <si>
+    <t>23.34 SAR</t>
+  </si>
+  <si>
+    <t>23,690.10 SAR</t>
+  </si>
+  <si>
+    <t>29.96 SAR</t>
+  </si>
+  <si>
+    <t>30,409.40 SAR</t>
+  </si>
+  <si>
+    <t>+6,719.30 SAR</t>
+  </si>
+  <si>
+    <t>+28.36%</t>
+  </si>
+  <si>
+    <t>8.11 SAR</t>
+  </si>
+  <si>
+    <t>24,330.00 SAR</t>
+  </si>
+  <si>
+    <t>38.46 SAR</t>
+  </si>
+  <si>
+    <t>115,380.00 SAR</t>
+  </si>
+  <si>
+    <t>+91,050.00 SAR</t>
+  </si>
+  <si>
+    <t>+374.23%</t>
+  </si>
+  <si>
+    <t>17.05 SAR</t>
+  </si>
+  <si>
+    <t>51,150.00 SAR</t>
+  </si>
+  <si>
+    <t>27.92 SAR</t>
+  </si>
+  <si>
+    <t>83,760.00 SAR</t>
+  </si>
+  <si>
+    <t>+32,610.00 SAR</t>
+  </si>
+  <si>
+    <t>+63.75%</t>
+  </si>
+  <si>
+    <t>22.28 SAR</t>
+  </si>
+  <si>
+    <t>66,104.76 SAR</t>
+  </si>
+  <si>
+    <t>33.82 SAR</t>
+  </si>
+  <si>
+    <t>100,343.94 SAR</t>
+  </si>
+  <si>
+    <t>+34,239.18 SAR</t>
+  </si>
+  <si>
+    <t>+51.80%</t>
+  </si>
+  <si>
+    <t>42.22 SAR</t>
+  </si>
+  <si>
+    <t>126,660.00 SAR</t>
+  </si>
+  <si>
+    <t>+720.00 SAR</t>
+  </si>
+  <si>
+    <t>+0.57%</t>
+  </si>
+  <si>
+    <t>10.90 SAR</t>
+  </si>
+  <si>
+    <t>102,460.00 SAR</t>
+  </si>
+  <si>
+    <t>+0.00 SAR</t>
+  </si>
+  <si>
+    <t>+0.00%</t>
+  </si>
+  <si>
+    <t>15.14 SAR</t>
+  </si>
+  <si>
+    <t>22,710.00 SAR</t>
+  </si>
+  <si>
+    <t>32,115.00 SAR</t>
+  </si>
+  <si>
+    <t>+9,405.00 SAR</t>
+  </si>
+  <si>
+    <t>+41.41%</t>
+  </si>
+  <si>
+    <t>AlBilad Saudi Growth</t>
+  </si>
+  <si>
+    <t>11.19 SAR</t>
+  </si>
+  <si>
+    <t>11,190.00 SAR</t>
+  </si>
+  <si>
+    <t>24.55 SAR</t>
+  </si>
+  <si>
+    <t>24,550.00 SAR</t>
+  </si>
+  <si>
+    <t>+13,360.00 SAR</t>
+  </si>
+  <si>
+    <t>+119.39%</t>
+  </si>
+  <si>
+    <t>8.50 SAR</t>
+  </si>
+  <si>
+    <t>82,867.50 SAR</t>
+  </si>
+  <si>
+    <t>38.95 SAR</t>
+  </si>
+  <si>
+    <t>379,762.50 SAR</t>
+  </si>
+  <si>
+    <t>+296,895.00 SAR</t>
+  </si>
+  <si>
+    <t>+358.28%</t>
+  </si>
+  <si>
+    <t>BSF Capital, Al Inma Capital</t>
+  </si>
+  <si>
+    <t>38.89 SAR</t>
+  </si>
+  <si>
+    <t>38,890.00 SAR</t>
+  </si>
+  <si>
+    <t>18.84 SAR</t>
+  </si>
+  <si>
+    <t>18,840.00 SAR</t>
+  </si>
+  <si>
+    <t>-20,050.00 SAR</t>
+  </si>
+  <si>
+    <t>-51.56%</t>
+  </si>
+  <si>
+    <t>4.71 SAR</t>
+  </si>
+  <si>
+    <t>39,893.70 SAR</t>
+  </si>
+  <si>
+    <t>24.28 SAR</t>
+  </si>
+  <si>
+    <t>205,651.60 SAR</t>
+  </si>
+  <si>
+    <t>+165,757.90 SAR</t>
+  </si>
+  <si>
+    <t>+415.50%</t>
+  </si>
+  <si>
+    <t>Al Inma Capital, BSF Capital</t>
+  </si>
+  <si>
+    <t>26.66 SAR</t>
+  </si>
+  <si>
+    <t>74,150.25 SAR</t>
+  </si>
+  <si>
+    <t>31.48 SAR</t>
+  </si>
+  <si>
+    <t>87,545.88 SAR</t>
+  </si>
+  <si>
+    <t>+13,395.63 SAR</t>
+  </si>
+  <si>
+    <t>+18.07%</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
+  </si>
+  <si>
+    <t>Current Value</t>
+  </si>
+  <si>
+    <t>27.11 SAR</t>
+  </si>
+  <si>
+    <t>106,027.21 SAR</t>
+  </si>
+  <si>
+    <t>12.55 SAR</t>
+  </si>
+  <si>
+    <t>132,352.30 SAR</t>
+  </si>
+  <si>
+    <t>22.42 SAR</t>
+  </si>
+  <si>
+    <t>82,191.72 SAR</t>
+  </si>
+  <si>
+    <t>26.71 SAR</t>
+  </si>
+  <si>
+    <t>40,065.00 SAR</t>
+  </si>
+  <si>
+    <t>25.72 SAR</t>
+  </si>
+  <si>
+    <t>95,729.84 SAR</t>
+  </si>
+  <si>
+    <t>35.68 SAR</t>
+  </si>
+  <si>
+    <t>71,360.00 SAR</t>
+  </si>
+  <si>
+    <t>62.14 SAR</t>
+  </si>
+  <si>
+    <t>186,420.00 SAR</t>
+  </si>
+  <si>
+    <t>23.97 SAR</t>
+  </si>
+  <si>
+    <t>25,432.17 SAR</t>
+  </si>
+  <si>
+    <t>59,950.00 SAR</t>
+  </si>
+  <si>
+    <t>27.29 SAR</t>
+  </si>
+  <si>
+    <t>40,935.00 SAR</t>
+  </si>
+  <si>
+    <t>46.43 SAR</t>
+  </si>
+  <si>
+    <t>29,993.78 SAR</t>
+  </si>
+  <si>
+    <t>14.78 SAR</t>
+  </si>
+  <si>
+    <t>14,780.00 SAR</t>
+  </si>
+  <si>
+    <t>7.86 SAR</t>
+  </si>
+  <si>
+    <t>74,670.00 SAR</t>
+  </si>
+  <si>
+    <t>2.32 SAR</t>
+  </si>
+  <si>
+    <t>15,776.00 SAR</t>
+  </si>
+  <si>
+    <t>5.66 SAR</t>
+  </si>
+  <si>
+    <t>22,640.00 SAR</t>
+  </si>
+  <si>
+    <t>42.50 SAR</t>
+  </si>
+  <si>
+    <t>127,500.00 SAR</t>
+  </si>
+  <si>
+    <t>10.89 SAR</t>
+  </si>
+  <si>
+    <t>102,366.00 SAR</t>
   </si>
 </sst>
 </file>
@@ -953,7 +1635,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -967,7 +1649,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -986,7 +1668,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -996,7 +1678,7 @@
       <name val="Avenir-heavy"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1036,6 +1718,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1122,7 +1810,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1197,6 +1885,39 @@
     <xf numFmtId="49" fontId="5" fillId="6" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1512,12 +2233,12 @@
       <selection activeCell="W264" sqref="R6:W264"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="15" max="20" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="18:23" ht="15" thickBot="1"/>
+    <row r="4" spans="18:23" ht="15.75" thickBot="1"/>
     <row r="5" spans="18:23" ht="18">
       <c r="S5" s="9"/>
       <c r="T5" s="10"/>
@@ -1545,7 +2266,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="7" spans="18:23" ht="28.5">
+    <row r="7" spans="18:23" ht="30">
       <c r="R7">
         <v>2</v>
       </c>
@@ -1565,7 +2286,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="8" spans="18:23" ht="28.5">
+    <row r="8" spans="18:23" ht="30">
       <c r="R8">
         <v>3</v>
       </c>
@@ -1585,7 +2306,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="9" spans="18:23" ht="28.5">
+    <row r="9" spans="18:23" ht="45">
       <c r="R9">
         <v>4</v>
       </c>
@@ -1645,7 +2366,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="12" spans="18:23" ht="28.5">
+    <row r="12" spans="18:23">
       <c r="R12">
         <v>7</v>
       </c>
@@ -1665,7 +2386,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="13" spans="18:23" ht="28.5">
+    <row r="13" spans="18:23" ht="30">
       <c r="R13">
         <v>8</v>
       </c>
@@ -1765,7 +2486,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="18" spans="18:23" ht="42.75">
+    <row r="18" spans="18:23" ht="45">
       <c r="R18">
         <v>13</v>
       </c>
@@ -1805,7 +2526,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="20" spans="18:23" ht="28.5">
+    <row r="20" spans="18:23" ht="30">
       <c r="R20">
         <v>15</v>
       </c>
@@ -1865,7 +2586,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="23" spans="18:23" ht="28.5">
+    <row r="23" spans="18:23" ht="30">
       <c r="R23">
         <v>18</v>
       </c>
@@ -1905,7 +2626,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="25" spans="18:23" ht="57">
+    <row r="25" spans="18:23" ht="60">
       <c r="R25">
         <v>20</v>
       </c>
@@ -2045,7 +2766,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="32" spans="18:23" ht="42.75">
+    <row r="32" spans="18:23" ht="45">
       <c r="R32">
         <v>27</v>
       </c>
@@ -2065,7 +2786,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="33" spans="18:23" ht="28.5">
+    <row r="33" spans="18:23" ht="30">
       <c r="R33">
         <v>28</v>
       </c>
@@ -2085,7 +2806,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="34" spans="18:23" ht="28.5">
+    <row r="34" spans="18:23">
       <c r="R34">
         <v>29</v>
       </c>
@@ -2105,7 +2826,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="35" spans="18:23" ht="28.5">
+    <row r="35" spans="18:23" ht="30">
       <c r="R35">
         <v>30</v>
       </c>
@@ -2205,7 +2926,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="40" spans="18:23" ht="28.5">
+    <row r="40" spans="18:23" ht="30">
       <c r="R40">
         <v>35</v>
       </c>
@@ -2225,7 +2946,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="41" spans="18:23" ht="28.5">
+    <row r="41" spans="18:23" ht="30">
       <c r="R41">
         <v>36</v>
       </c>
@@ -2265,7 +2986,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="43" spans="18:23" ht="28.5">
+    <row r="43" spans="18:23" ht="30">
       <c r="R43">
         <v>38</v>
       </c>
@@ -2285,7 +3006,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="44" spans="18:23" ht="28.5">
+    <row r="44" spans="18:23" ht="30">
       <c r="R44">
         <v>39</v>
       </c>
@@ -2305,7 +3026,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="45" spans="18:23" ht="42.75">
+    <row r="45" spans="18:23" ht="45">
       <c r="R45">
         <v>40</v>
       </c>
@@ -2365,7 +3086,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="48" spans="18:23" ht="28.5">
+    <row r="48" spans="18:23" ht="30">
       <c r="R48">
         <v>43</v>
       </c>
@@ -2425,7 +3146,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="51" spans="18:23" ht="28.5">
+    <row r="51" spans="18:23" ht="30">
       <c r="R51">
         <v>46</v>
       </c>
@@ -2545,7 +3266,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="57" spans="18:23" ht="28.5">
+    <row r="57" spans="18:23" ht="30">
       <c r="R57">
         <v>52</v>
       </c>
@@ -2565,7 +3286,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="58" spans="18:23" ht="28.5">
+    <row r="58" spans="18:23" ht="30">
       <c r="R58">
         <v>53</v>
       </c>
@@ -2585,7 +3306,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="59" spans="18:23" ht="42.75">
+    <row r="59" spans="18:23" ht="45">
       <c r="R59">
         <v>54</v>
       </c>
@@ -2665,7 +3386,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="63" spans="18:23" ht="42.75">
+    <row r="63" spans="18:23" ht="45">
       <c r="R63">
         <v>58</v>
       </c>
@@ -2685,7 +3406,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="64" spans="18:23" ht="28.5">
+    <row r="64" spans="18:23" ht="30">
       <c r="R64">
         <v>59</v>
       </c>
@@ -2705,7 +3426,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="65" spans="18:23">
+    <row r="65" spans="18:23" ht="30">
       <c r="R65">
         <v>60</v>
       </c>
@@ -2725,7 +3446,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="66" spans="18:23" ht="28.5">
+    <row r="66" spans="18:23" ht="30">
       <c r="R66">
         <v>61</v>
       </c>
@@ -2805,7 +3526,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="70" spans="18:23" ht="28.5">
+    <row r="70" spans="18:23" ht="30">
       <c r="R70">
         <v>65</v>
       </c>
@@ -2825,7 +3546,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="71" spans="18:23" ht="28.5">
+    <row r="71" spans="18:23" ht="30">
       <c r="R71">
         <v>66</v>
       </c>
@@ -2885,7 +3606,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="74" spans="18:23" ht="28.5">
+    <row r="74" spans="18:23" ht="30">
       <c r="R74">
         <v>69</v>
       </c>
@@ -2905,7 +3626,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="75" spans="18:23" ht="28.5">
+    <row r="75" spans="18:23" ht="30">
       <c r="R75">
         <v>70</v>
       </c>
@@ -2945,7 +3666,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="77" spans="18:23" ht="28.5">
+    <row r="77" spans="18:23" ht="30">
       <c r="R77">
         <v>72</v>
       </c>
@@ -2985,7 +3706,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="79" spans="18:23" ht="28.5">
+    <row r="79" spans="18:23" ht="30">
       <c r="R79">
         <v>74</v>
       </c>
@@ -3045,7 +3766,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="82" spans="18:23" ht="28.5">
+    <row r="82" spans="18:23" ht="45">
       <c r="R82">
         <v>77</v>
       </c>
@@ -3105,7 +3826,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="85" spans="18:23" ht="28.5">
+    <row r="85" spans="18:23" ht="30">
       <c r="R85">
         <v>80</v>
       </c>
@@ -3265,7 +3986,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="93" spans="18:23" ht="28.5">
+    <row r="93" spans="18:23">
       <c r="R93">
         <v>88</v>
       </c>
@@ -3305,7 +4026,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="95" spans="18:23" ht="28.5">
+    <row r="95" spans="18:23" ht="30">
       <c r="R95">
         <v>90</v>
       </c>
@@ -3365,7 +4086,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="98" spans="18:23" ht="28.5">
+    <row r="98" spans="18:23" ht="30">
       <c r="R98">
         <v>93</v>
       </c>
@@ -3405,7 +4126,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="100" spans="18:23" ht="28.5">
+    <row r="100" spans="18:23" ht="30">
       <c r="R100">
         <v>95</v>
       </c>
@@ -3465,7 +4186,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="103" spans="18:23" ht="28.5">
+    <row r="103" spans="18:23" ht="30">
       <c r="R103">
         <v>98</v>
       </c>
@@ -3545,7 +4266,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="107" spans="18:23" ht="28.5">
+    <row r="107" spans="18:23" ht="30">
       <c r="R107">
         <v>102</v>
       </c>
@@ -3565,7 +4286,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="108" spans="18:23" ht="28.5">
+    <row r="108" spans="18:23" ht="30">
       <c r="R108">
         <v>103</v>
       </c>
@@ -3605,7 +4326,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="110" spans="18:23" ht="28.5">
+    <row r="110" spans="18:23" ht="30">
       <c r="R110">
         <v>105</v>
       </c>
@@ -3645,7 +4366,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="112" spans="18:23" ht="28.5">
+    <row r="112" spans="18:23" ht="30">
       <c r="R112">
         <v>107</v>
       </c>
@@ -3665,7 +4386,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="113" spans="18:23" ht="28.5">
+    <row r="113" spans="18:23" ht="30">
       <c r="R113">
         <v>108</v>
       </c>
@@ -3765,7 +4486,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="118" spans="18:23" ht="28.5">
+    <row r="118" spans="18:23" ht="30">
       <c r="R118">
         <v>113</v>
       </c>
@@ -3805,7 +4526,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="120" spans="18:23" ht="28.5">
+    <row r="120" spans="18:23" ht="30">
       <c r="R120">
         <v>115</v>
       </c>
@@ -3825,7 +4546,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="121" spans="18:23" ht="42.75">
+    <row r="121" spans="18:23" ht="30">
       <c r="R121">
         <v>116</v>
       </c>
@@ -3845,7 +4566,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="122" spans="18:23" ht="28.5">
+    <row r="122" spans="18:23" ht="30">
       <c r="R122">
         <v>117</v>
       </c>
@@ -3865,7 +4586,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="123" spans="18:23" ht="28.5">
+    <row r="123" spans="18:23" ht="30">
       <c r="R123">
         <v>118</v>
       </c>
@@ -3885,7 +4606,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="124" spans="18:23" ht="42.75">
+    <row r="124" spans="18:23" ht="45">
       <c r="R124">
         <v>119</v>
       </c>
@@ -3905,7 +4626,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="125" spans="18:23" ht="42.75">
+    <row r="125" spans="18:23" ht="45">
       <c r="R125">
         <v>120</v>
       </c>
@@ -3925,7 +4646,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="126" spans="18:23" ht="28.5">
+    <row r="126" spans="18:23" ht="45">
       <c r="R126">
         <v>121</v>
       </c>
@@ -3965,7 +4686,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="128" spans="18:23" ht="28.5">
+    <row r="128" spans="18:23" ht="30">
       <c r="R128">
         <v>123</v>
       </c>
@@ -3985,7 +4706,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="129" spans="18:23" ht="28.5">
+    <row r="129" spans="18:23" ht="30">
       <c r="R129">
         <v>124</v>
       </c>
@@ -4005,7 +4726,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="130" spans="18:23" ht="28.5">
+    <row r="130" spans="18:23" ht="30">
       <c r="R130">
         <v>125</v>
       </c>
@@ -4045,7 +4766,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="132" spans="18:23" ht="28.5">
+    <row r="132" spans="18:23" ht="30">
       <c r="R132">
         <v>127</v>
       </c>
@@ -4085,7 +4806,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="134" spans="18:23" ht="28.5">
+    <row r="134" spans="18:23" ht="30">
       <c r="R134">
         <v>129</v>
       </c>
@@ -4105,7 +4826,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="135" spans="18:23">
+    <row r="135" spans="18:23" ht="30">
       <c r="R135">
         <v>130</v>
       </c>
@@ -4125,7 +4846,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="136" spans="18:23">
+    <row r="136" spans="18:23" ht="30">
       <c r="R136">
         <v>131</v>
       </c>
@@ -4165,7 +4886,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="138" spans="18:23" ht="28.5">
+    <row r="138" spans="18:23" ht="30">
       <c r="R138">
         <v>133</v>
       </c>
@@ -4185,7 +4906,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="139" spans="18:23" ht="28.5">
+    <row r="139" spans="18:23" ht="30">
       <c r="R139">
         <v>134</v>
       </c>
@@ -4205,7 +4926,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="140" spans="18:23" ht="28.5">
+    <row r="140" spans="18:23" ht="30">
       <c r="R140">
         <v>135</v>
       </c>
@@ -4225,7 +4946,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="141" spans="18:23" ht="28.5">
+    <row r="141" spans="18:23" ht="30">
       <c r="R141">
         <v>136</v>
       </c>
@@ -4265,7 +4986,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="143" spans="18:23" ht="28.5">
+    <row r="143" spans="18:23" ht="45">
       <c r="R143">
         <v>138</v>
       </c>
@@ -4385,7 +5106,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="149" spans="18:23" ht="28.5">
+    <row r="149" spans="18:23" ht="30">
       <c r="R149">
         <v>144</v>
       </c>
@@ -4425,7 +5146,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="151" spans="18:23" ht="28.5">
+    <row r="151" spans="18:23" ht="30">
       <c r="R151">
         <v>146</v>
       </c>
@@ -4445,7 +5166,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="152" spans="18:23" ht="28.5">
+    <row r="152" spans="18:23" ht="30">
       <c r="R152">
         <v>147</v>
       </c>
@@ -4485,7 +5206,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="154" spans="18:23" ht="28.5">
+    <row r="154" spans="18:23" ht="30">
       <c r="R154">
         <v>149</v>
       </c>
@@ -4505,7 +5226,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="155" spans="18:23" ht="28.5">
+    <row r="155" spans="18:23" ht="30">
       <c r="R155">
         <v>150</v>
       </c>
@@ -4525,7 +5246,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="156" spans="18:23" ht="28.5">
+    <row r="156" spans="18:23" ht="30">
       <c r="R156">
         <v>151</v>
       </c>
@@ -4565,7 +5286,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="158" spans="18:23" ht="28.5">
+    <row r="158" spans="18:23" ht="30">
       <c r="R158">
         <v>153</v>
       </c>
@@ -4585,7 +5306,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="159" spans="18:23" ht="42.75">
+    <row r="159" spans="18:23" ht="45">
       <c r="R159">
         <v>154</v>
       </c>
@@ -4605,7 +5326,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="160" spans="18:23" ht="42.75">
+    <row r="160" spans="18:23" ht="45">
       <c r="R160">
         <v>155</v>
       </c>
@@ -4625,7 +5346,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="161" spans="18:23" ht="42.75">
+    <row r="161" spans="18:23" ht="45">
       <c r="R161">
         <v>156</v>
       </c>
@@ -4645,7 +5366,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="162" spans="18:23" ht="28.5">
+    <row r="162" spans="18:23" ht="30">
       <c r="R162">
         <v>157</v>
       </c>
@@ -4665,7 +5386,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="163" spans="18:23" ht="28.5">
+    <row r="163" spans="18:23" ht="30">
       <c r="R163">
         <v>158</v>
       </c>
@@ -4685,7 +5406,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="164" spans="18:23" ht="42.75">
+    <row r="164" spans="18:23" ht="45">
       <c r="R164">
         <v>159</v>
       </c>
@@ -4705,7 +5426,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="165" spans="18:23" ht="28.5">
+    <row r="165" spans="18:23" ht="30">
       <c r="R165">
         <v>160</v>
       </c>
@@ -4725,7 +5446,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="166" spans="18:23" ht="42.75">
+    <row r="166" spans="18:23" ht="45">
       <c r="R166">
         <v>161</v>
       </c>
@@ -4745,7 +5466,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="167" spans="18:23" ht="28.5">
+    <row r="167" spans="18:23" ht="30">
       <c r="R167">
         <v>162</v>
       </c>
@@ -4965,7 +5686,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="178" spans="18:23" ht="42.75">
+    <row r="178" spans="18:23" ht="30">
       <c r="R178">
         <v>173</v>
       </c>
@@ -5085,7 +5806,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="184" spans="18:23" ht="28.5">
+    <row r="184" spans="18:23">
       <c r="R184">
         <v>179</v>
       </c>
@@ -5105,7 +5826,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="185" spans="18:23" ht="28.5">
+    <row r="185" spans="18:23" ht="30">
       <c r="R185">
         <v>180</v>
       </c>
@@ -5125,7 +5846,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="186" spans="18:23" ht="28.5">
+    <row r="186" spans="18:23" ht="30">
       <c r="R186">
         <v>181</v>
       </c>
@@ -5145,7 +5866,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="187" spans="18:23" ht="28.5">
+    <row r="187" spans="18:23" ht="30">
       <c r="R187">
         <v>182</v>
       </c>
@@ -5165,7 +5886,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="188" spans="18:23" ht="28.5">
+    <row r="188" spans="18:23" ht="30">
       <c r="R188">
         <v>183</v>
       </c>
@@ -5185,7 +5906,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="189" spans="18:23" ht="28.5">
+    <row r="189" spans="18:23" ht="30">
       <c r="R189">
         <v>184</v>
       </c>
@@ -5205,7 +5926,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="190" spans="18:23" ht="42.75">
+    <row r="190" spans="18:23" ht="45">
       <c r="R190">
         <v>185</v>
       </c>
@@ -5225,7 +5946,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="191" spans="18:23" ht="28.5">
+    <row r="191" spans="18:23" ht="30">
       <c r="R191">
         <v>186</v>
       </c>
@@ -5245,7 +5966,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="192" spans="18:23" ht="28.5">
+    <row r="192" spans="18:23" ht="30">
       <c r="R192">
         <v>187</v>
       </c>
@@ -5305,7 +6026,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="195" spans="18:23" ht="28.5">
+    <row r="195" spans="18:23" ht="30">
       <c r="R195">
         <v>190</v>
       </c>
@@ -5345,7 +6066,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="197" spans="18:23" ht="42.75">
+    <row r="197" spans="18:23" ht="45">
       <c r="R197">
         <v>192</v>
       </c>
@@ -5405,7 +6126,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="200" spans="18:23" ht="28.5">
+    <row r="200" spans="18:23" ht="30">
       <c r="R200">
         <v>195</v>
       </c>
@@ -5425,7 +6146,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="201" spans="18:23" ht="42.75">
+    <row r="201" spans="18:23" ht="45">
       <c r="R201">
         <v>196</v>
       </c>
@@ -5465,7 +6186,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="203" spans="18:23" ht="28.5">
+    <row r="203" spans="18:23">
       <c r="R203">
         <v>198</v>
       </c>
@@ -5485,7 +6206,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="204" spans="18:23" ht="28.5">
+    <row r="204" spans="18:23" ht="30">
       <c r="R204">
         <v>199</v>
       </c>
@@ -5505,7 +6226,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="205" spans="18:23" ht="28.5">
+    <row r="205" spans="18:23" ht="30">
       <c r="R205">
         <v>200</v>
       </c>
@@ -5565,7 +6286,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="208" spans="18:23" ht="42.75">
+    <row r="208" spans="18:23" ht="30">
       <c r="R208">
         <v>203</v>
       </c>
@@ -5625,7 +6346,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="211" spans="18:23" ht="28.5">
+    <row r="211" spans="18:23" ht="30">
       <c r="R211">
         <v>206</v>
       </c>
@@ -5645,7 +6366,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="212" spans="18:23" ht="42.75">
+    <row r="212" spans="18:23" ht="45">
       <c r="R212">
         <v>207</v>
       </c>
@@ -5725,7 +6446,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="216" spans="18:23" ht="28.5">
+    <row r="216" spans="18:23" ht="30">
       <c r="R216">
         <v>211</v>
       </c>
@@ -5745,7 +6466,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="217" spans="18:23" ht="28.5">
+    <row r="217" spans="18:23" ht="30">
       <c r="R217">
         <v>212</v>
       </c>
@@ -5845,7 +6566,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="222" spans="18:23" ht="42.75">
+    <row r="222" spans="18:23" ht="30">
       <c r="R222">
         <v>217</v>
       </c>
@@ -5865,7 +6586,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="223" spans="18:23">
+    <row r="223" spans="18:23" ht="30">
       <c r="R223">
         <v>218</v>
       </c>
@@ -5885,7 +6606,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="224" spans="18:23" ht="42.75">
+    <row r="224" spans="18:23" ht="45">
       <c r="R224">
         <v>219</v>
       </c>
@@ -5945,7 +6666,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="227" spans="18:23" ht="28.5">
+    <row r="227" spans="18:23" ht="30">
       <c r="R227">
         <v>222</v>
       </c>
@@ -5965,7 +6686,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="228" spans="18:23">
+    <row r="228" spans="18:23" ht="30">
       <c r="R228">
         <v>223</v>
       </c>
@@ -5985,7 +6706,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="229" spans="18:23">
+    <row r="229" spans="18:23" ht="30">
       <c r="R229">
         <v>224</v>
       </c>
@@ -6005,7 +6726,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="230" spans="18:23" ht="42.75">
+    <row r="230" spans="18:23" ht="45">
       <c r="R230">
         <v>225</v>
       </c>
@@ -6025,7 +6746,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="231" spans="18:23" ht="28.5">
+    <row r="231" spans="18:23" ht="30">
       <c r="R231">
         <v>226</v>
       </c>
@@ -6045,7 +6766,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="232" spans="18:23" ht="28.5">
+    <row r="232" spans="18:23" ht="30">
       <c r="R232">
         <v>227</v>
       </c>
@@ -6065,7 +6786,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="233" spans="18:23" ht="57">
+    <row r="233" spans="18:23" ht="60">
       <c r="R233">
         <v>228</v>
       </c>
@@ -6085,7 +6806,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="234" spans="18:23" ht="28.5">
+    <row r="234" spans="18:23" ht="30">
       <c r="R234">
         <v>229</v>
       </c>
@@ -6105,7 +6826,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="235" spans="18:23" ht="42.75">
+    <row r="235" spans="18:23" ht="45">
       <c r="R235">
         <v>230</v>
       </c>
@@ -6125,7 +6846,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="236" spans="18:23" ht="28.5">
+    <row r="236" spans="18:23" ht="30">
       <c r="R236">
         <v>231</v>
       </c>
@@ -6145,7 +6866,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="237" spans="18:23" ht="28.5">
+    <row r="237" spans="18:23" ht="30">
       <c r="R237">
         <v>232</v>
       </c>
@@ -6165,7 +6886,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="238" spans="18:23" ht="42.75">
+    <row r="238" spans="18:23" ht="45">
       <c r="R238">
         <v>233</v>
       </c>
@@ -6185,7 +6906,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="239" spans="18:23" ht="28.5">
+    <row r="239" spans="18:23" ht="30">
       <c r="R239">
         <v>234</v>
       </c>
@@ -6205,7 +6926,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="240" spans="18:23" ht="28.5">
+    <row r="240" spans="18:23" ht="30">
       <c r="R240">
         <v>235</v>
       </c>
@@ -6225,7 +6946,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="241" spans="18:23" ht="28.5">
+    <row r="241" spans="18:23" ht="30">
       <c r="R241">
         <v>236</v>
       </c>
@@ -6245,7 +6966,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="242" spans="18:23" ht="42.75">
+    <row r="242" spans="18:23" ht="45">
       <c r="R242">
         <v>237</v>
       </c>
@@ -6265,7 +6986,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="243" spans="18:23" ht="42.75">
+    <row r="243" spans="18:23" ht="45">
       <c r="R243">
         <v>238</v>
       </c>
@@ -6285,7 +7006,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="244" spans="18:23" ht="42.75">
+    <row r="244" spans="18:23" ht="45">
       <c r="R244">
         <v>239</v>
       </c>
@@ -6305,7 +7026,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="245" spans="18:23" ht="28.5">
+    <row r="245" spans="18:23" ht="30">
       <c r="R245">
         <v>240</v>
       </c>
@@ -6325,7 +7046,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="246" spans="18:23" ht="28.5">
+    <row r="246" spans="18:23" ht="30">
       <c r="R246">
         <v>241</v>
       </c>
@@ -6345,7 +7066,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="247" spans="18:23" ht="42.75">
+    <row r="247" spans="18:23" ht="30">
       <c r="R247">
         <v>242</v>
       </c>
@@ -6365,7 +7086,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="248" spans="18:23" ht="57">
+    <row r="248" spans="18:23" ht="45">
       <c r="R248">
         <v>243</v>
       </c>
@@ -6385,7 +7106,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="249" spans="18:23" ht="42.75">
+    <row r="249" spans="18:23" ht="45">
       <c r="R249">
         <v>244</v>
       </c>
@@ -6405,7 +7126,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="250" spans="18:23" ht="28.5">
+    <row r="250" spans="18:23" ht="30">
       <c r="R250">
         <v>245</v>
       </c>
@@ -6485,7 +7206,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="254" spans="18:23" ht="28.5">
+    <row r="254" spans="18:23" ht="30">
       <c r="R254">
         <v>249</v>
       </c>
@@ -6525,7 +7246,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="256" spans="18:23" ht="28.5">
+    <row r="256" spans="18:23" ht="30">
       <c r="R256">
         <v>251</v>
       </c>
@@ -6545,7 +7266,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="257" spans="18:23" ht="42.75">
+    <row r="257" spans="18:23" ht="45">
       <c r="R257">
         <v>252</v>
       </c>
@@ -6585,7 +7306,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="259" spans="18:23" ht="28.5">
+    <row r="259" spans="18:23" ht="30">
       <c r="R259">
         <v>254</v>
       </c>
@@ -6605,7 +7326,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="260" spans="18:23" ht="42.75">
+    <row r="260" spans="18:23" ht="30">
       <c r="R260">
         <v>255</v>
       </c>
@@ -6975,21 +7696,22 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D13" sqref="D2:D13"/>
+    <sheetView topLeftCell="A24" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="34.625" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="6" width="12" customWidth="1"/>
+    <col min="4" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15">
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7048,7 +7770,7 @@
         <v>13.67</v>
       </c>
       <c r="F3" s="3">
-        <f t="shared" ref="F3:F40" si="0">+D3*E3</f>
+        <f t="shared" ref="F3:F41" si="0">+D3*E3</f>
         <v>144163.82</v>
       </c>
       <c r="G3" s="4" t="s">
@@ -7937,24 +8659,2140 @@
       </c>
     </row>
     <row r="41" spans="1:7">
+      <c r="A41">
+        <v>37</v>
+      </c>
+      <c r="B41" t="s">
+        <v>301</v>
+      </c>
+      <c r="C41">
+        <v>4007</v>
+      </c>
       <c r="D41">
-        <f>SUM(D2:D40)</f>
-        <v>126367</v>
+        <v>1000</v>
       </c>
       <c r="E41">
-        <f>SUM(E2:E40)</f>
-        <v>962.80000000000007</v>
+        <v>38.89</v>
+      </c>
+      <c r="F41" s="3">
+        <f t="shared" si="0"/>
+        <v>38890</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="D44">
+        <f>SUM(D2:D41)</f>
+        <v>127367</v>
+      </c>
+      <c r="E44">
+        <f>SUM(E2:E41)</f>
+        <v>1001.69</v>
+      </c>
+      <c r="F44" s="28">
+        <f>SUM(F2:F41)</f>
+        <v>2300910.58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="F45">
+        <v>2262020.58</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G41" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G40">
     <sortCondition ref="C2:C40"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44E751F-DD30-4116-B541-E478FC44B037}">
+  <dimension ref="F5:V43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24:Q24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="8" max="8" width="22.28515625" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="40"/>
+    <col min="14" max="14" width="15.5703125" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" customWidth="1"/>
+    <col min="17" max="19" width="14.7109375" customWidth="1"/>
+    <col min="21" max="21" width="12.28515625" customWidth="1"/>
+    <col min="22" max="22" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="6:22">
+      <c r="L5" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="6" spans="6:22" ht="30">
+      <c r="F6" s="29">
+        <v>1</v>
+      </c>
+      <c r="G6" s="29">
+        <v>1010</v>
+      </c>
+      <c r="H6" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="I6" s="30">
+        <v>3911</v>
+      </c>
+      <c r="J6" s="29" t="s">
+        <v>302</v>
+      </c>
+      <c r="K6" s="29" t="s">
+        <v>303</v>
+      </c>
+      <c r="L6" s="33">
+        <f>VALUE(SUBSTITUTE(K6, " SAR", ""))</f>
+        <v>108582.98</v>
+      </c>
+      <c r="M6" s="36" t="s">
+        <v>494</v>
+      </c>
+      <c r="N6" s="29" t="s">
+        <v>495</v>
+      </c>
+      <c r="O6" s="33">
+        <f>VALUE(SUBSTITUTE(N6, " SAR", ""))</f>
+        <v>106027.21</v>
+      </c>
+      <c r="P6" s="35">
+        <f>+O6-L6</f>
+        <v>-2555.7699999999895</v>
+      </c>
+      <c r="Q6" s="29" t="s">
+        <v>304</v>
+      </c>
+      <c r="R6" s="29"/>
+      <c r="S6" s="32">
+        <f>VALUE(SUBSTITUTE(Q6, " SAR", ""))</f>
+        <v>-2712.21</v>
+      </c>
+      <c r="T6" s="29" t="s">
+        <v>305</v>
+      </c>
+      <c r="U6" s="31">
+        <v>45892</v>
+      </c>
+      <c r="V6" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="6:22" ht="30">
+      <c r="F7" s="29">
+        <v>2</v>
+      </c>
+      <c r="G7" s="29">
+        <v>1020</v>
+      </c>
+      <c r="H7" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="30">
+        <v>10546</v>
+      </c>
+      <c r="J7" s="29" t="s">
+        <v>306</v>
+      </c>
+      <c r="K7" s="29" t="s">
+        <v>307</v>
+      </c>
+      <c r="L7" s="33">
+        <f t="shared" ref="L7:L42" si="0">VALUE(SUBSTITUTE(K7, " SAR", ""))</f>
+        <v>144163.82</v>
+      </c>
+      <c r="M7" s="36" t="s">
+        <v>496</v>
+      </c>
+      <c r="N7" s="29" t="s">
+        <v>497</v>
+      </c>
+      <c r="O7" s="33">
+        <f t="shared" ref="O7:O42" si="1">VALUE(SUBSTITUTE(N7, " SAR", ""))</f>
+        <v>132352.29999999999</v>
+      </c>
+      <c r="P7" s="35">
+        <f t="shared" ref="P7:P42" si="2">+O7-L7</f>
+        <v>-11811.520000000019</v>
+      </c>
+      <c r="Q7" s="29" t="s">
+        <v>308</v>
+      </c>
+      <c r="R7" s="29"/>
+      <c r="S7" s="32">
+        <f t="shared" ref="S7:S42" si="3">VALUE(SUBSTITUTE(Q7, " SAR", ""))</f>
+        <v>-11916.98</v>
+      </c>
+      <c r="T7" s="29" t="s">
+        <v>309</v>
+      </c>
+      <c r="U7" s="31">
+        <v>45657</v>
+      </c>
+      <c r="V7" s="29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="6:22" ht="30">
+      <c r="F8" s="29">
+        <v>3</v>
+      </c>
+      <c r="G8" s="29">
+        <v>1080</v>
+      </c>
+      <c r="H8" s="29" t="s">
+        <v>209</v>
+      </c>
+      <c r="I8" s="30">
+        <v>3666</v>
+      </c>
+      <c r="J8" s="29" t="s">
+        <v>310</v>
+      </c>
+      <c r="K8" s="29" t="s">
+        <v>311</v>
+      </c>
+      <c r="L8" s="33">
+        <f t="shared" si="0"/>
+        <v>79845.48</v>
+      </c>
+      <c r="M8" s="36" t="s">
+        <v>498</v>
+      </c>
+      <c r="N8" s="29" t="s">
+        <v>499</v>
+      </c>
+      <c r="O8" s="33">
+        <f t="shared" si="1"/>
+        <v>82191.72</v>
+      </c>
+      <c r="P8" s="35">
+        <f t="shared" si="2"/>
+        <v>2346.2400000000052</v>
+      </c>
+      <c r="Q8" s="29" t="s">
+        <v>312</v>
+      </c>
+      <c r="R8" s="29"/>
+      <c r="S8" s="32">
+        <f t="shared" si="3"/>
+        <v>2236.2600000000002</v>
+      </c>
+      <c r="T8" s="29" t="s">
+        <v>313</v>
+      </c>
+      <c r="U8" s="31">
+        <v>45657</v>
+      </c>
+      <c r="V8" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="6:22" ht="30">
+      <c r="F9" s="29">
+        <v>4</v>
+      </c>
+      <c r="G9" s="29">
+        <v>1140</v>
+      </c>
+      <c r="H9" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="30">
+        <v>1500</v>
+      </c>
+      <c r="J9" s="29" t="s">
+        <v>314</v>
+      </c>
+      <c r="K9" s="29" t="s">
+        <v>315</v>
+      </c>
+      <c r="L9" s="33">
+        <f t="shared" si="0"/>
+        <v>40965</v>
+      </c>
+      <c r="M9" s="36" t="s">
+        <v>500</v>
+      </c>
+      <c r="N9" s="29" t="s">
+        <v>501</v>
+      </c>
+      <c r="O9" s="33">
+        <f t="shared" si="1"/>
+        <v>40065</v>
+      </c>
+      <c r="P9" s="35">
+        <f t="shared" si="2"/>
+        <v>-900</v>
+      </c>
+      <c r="Q9" s="29" t="s">
+        <v>316</v>
+      </c>
+      <c r="R9" s="29"/>
+      <c r="S9" s="32">
+        <f t="shared" si="3"/>
+        <v>-990</v>
+      </c>
+      <c r="T9" s="29" t="s">
+        <v>317</v>
+      </c>
+      <c r="U9" s="31">
+        <v>45657</v>
+      </c>
+      <c r="V9" s="29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="6:22" ht="30">
+      <c r="F10" s="29">
+        <v>5</v>
+      </c>
+      <c r="G10" s="29">
+        <v>1150</v>
+      </c>
+      <c r="H10" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="30">
+        <v>3722</v>
+      </c>
+      <c r="J10" s="29" t="s">
+        <v>318</v>
+      </c>
+      <c r="K10" s="29" t="s">
+        <v>319</v>
+      </c>
+      <c r="L10" s="33">
+        <f t="shared" si="0"/>
+        <v>100568.44</v>
+      </c>
+      <c r="M10" s="36" t="s">
+        <v>502</v>
+      </c>
+      <c r="N10" s="29" t="s">
+        <v>503</v>
+      </c>
+      <c r="O10" s="33">
+        <f t="shared" si="1"/>
+        <v>95729.84</v>
+      </c>
+      <c r="P10" s="35">
+        <f t="shared" si="2"/>
+        <v>-4838.6000000000058</v>
+      </c>
+      <c r="Q10" s="29" t="s">
+        <v>320</v>
+      </c>
+      <c r="R10" s="29"/>
+      <c r="S10" s="32">
+        <f t="shared" si="3"/>
+        <v>-4987.4799999999996</v>
+      </c>
+      <c r="T10" s="29" t="s">
+        <v>321</v>
+      </c>
+      <c r="U10" s="31">
+        <v>45657</v>
+      </c>
+      <c r="V10" s="29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="6:22" ht="30">
+      <c r="F11" s="29">
+        <v>6</v>
+      </c>
+      <c r="G11" s="29">
+        <v>1180</v>
+      </c>
+      <c r="H11" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="I11" s="30">
+        <v>2000</v>
+      </c>
+      <c r="J11" s="29" t="s">
+        <v>322</v>
+      </c>
+      <c r="K11" s="29" t="s">
+        <v>323</v>
+      </c>
+      <c r="L11" s="33">
+        <f t="shared" si="0"/>
+        <v>72080</v>
+      </c>
+      <c r="M11" s="36" t="s">
+        <v>504</v>
+      </c>
+      <c r="N11" s="29" t="s">
+        <v>505</v>
+      </c>
+      <c r="O11" s="33">
+        <f t="shared" si="1"/>
+        <v>71360</v>
+      </c>
+      <c r="P11" s="35">
+        <f t="shared" si="2"/>
+        <v>-720</v>
+      </c>
+      <c r="Q11" s="29" t="s">
+        <v>324</v>
+      </c>
+      <c r="R11" s="29"/>
+      <c r="S11" s="32">
+        <f t="shared" si="3"/>
+        <v>-800</v>
+      </c>
+      <c r="T11" s="29" t="s">
+        <v>325</v>
+      </c>
+      <c r="U11" s="31">
+        <v>45657</v>
+      </c>
+      <c r="V11" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="6:22" ht="30">
+      <c r="F12" s="29">
+        <v>7</v>
+      </c>
+      <c r="G12" s="29">
+        <v>1304</v>
+      </c>
+      <c r="H12" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" s="30">
+        <v>1000</v>
+      </c>
+      <c r="J12" s="29" t="s">
+        <v>326</v>
+      </c>
+      <c r="K12" s="29" t="s">
+        <v>327</v>
+      </c>
+      <c r="L12" s="33">
+        <f t="shared" si="0"/>
+        <v>38690</v>
+      </c>
+      <c r="M12" s="36" t="s">
+        <v>328</v>
+      </c>
+      <c r="N12" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="O12" s="33">
+        <f t="shared" si="1"/>
+        <v>34970</v>
+      </c>
+      <c r="P12" s="35">
+        <f t="shared" si="2"/>
+        <v>-3720</v>
+      </c>
+      <c r="Q12" s="29" t="s">
+        <v>330</v>
+      </c>
+      <c r="R12" s="29"/>
+      <c r="S12" s="32">
+        <f t="shared" si="3"/>
+        <v>-3720</v>
+      </c>
+      <c r="T12" s="29" t="s">
+        <v>331</v>
+      </c>
+      <c r="U12" s="31">
+        <v>45657</v>
+      </c>
+      <c r="V12" s="29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="6:22" ht="30">
+      <c r="F13" s="29">
+        <v>8</v>
+      </c>
+      <c r="G13" s="29">
+        <v>1120</v>
+      </c>
+      <c r="H13" s="29" t="s">
+        <v>210</v>
+      </c>
+      <c r="I13" s="29">
+        <v>500</v>
+      </c>
+      <c r="J13" s="29" t="s">
+        <v>332</v>
+      </c>
+      <c r="K13" s="29" t="s">
+        <v>333</v>
+      </c>
+      <c r="L13" s="33">
+        <f t="shared" si="0"/>
+        <v>46300</v>
+      </c>
+      <c r="M13" s="36" t="s">
+        <v>334</v>
+      </c>
+      <c r="N13" s="29" t="s">
+        <v>335</v>
+      </c>
+      <c r="O13" s="33">
+        <f t="shared" si="1"/>
+        <v>48495</v>
+      </c>
+      <c r="P13" s="35">
+        <f t="shared" si="2"/>
+        <v>2195</v>
+      </c>
+      <c r="Q13" s="29" t="s">
+        <v>336</v>
+      </c>
+      <c r="R13" s="29"/>
+      <c r="S13" s="32">
+        <f t="shared" si="3"/>
+        <v>2195</v>
+      </c>
+      <c r="T13" s="29" t="s">
+        <v>337</v>
+      </c>
+      <c r="U13" s="31">
+        <v>45886</v>
+      </c>
+      <c r="V13" s="29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="6:22" ht="30">
+      <c r="F14" s="29">
+        <v>9</v>
+      </c>
+      <c r="G14" s="29">
+        <v>2010</v>
+      </c>
+      <c r="H14" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" s="30">
+        <v>3000</v>
+      </c>
+      <c r="J14" s="29" t="s">
+        <v>338</v>
+      </c>
+      <c r="K14" s="29" t="s">
+        <v>339</v>
+      </c>
+      <c r="L14" s="33">
+        <f t="shared" si="0"/>
+        <v>215910</v>
+      </c>
+      <c r="M14" s="36" t="s">
+        <v>506</v>
+      </c>
+      <c r="N14" s="29" t="s">
+        <v>507</v>
+      </c>
+      <c r="O14" s="33">
+        <f t="shared" si="1"/>
+        <v>186420</v>
+      </c>
+      <c r="P14" s="35">
+        <f t="shared" si="2"/>
+        <v>-29490</v>
+      </c>
+      <c r="Q14" s="29" t="s">
+        <v>340</v>
+      </c>
+      <c r="R14" s="29"/>
+      <c r="S14" s="32">
+        <f t="shared" si="3"/>
+        <v>-29640</v>
+      </c>
+      <c r="T14" s="29" t="s">
+        <v>341</v>
+      </c>
+      <c r="U14" s="31">
+        <v>45657</v>
+      </c>
+      <c r="V14" s="29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="6:22" ht="30">
+      <c r="F15" s="29">
+        <v>10</v>
+      </c>
+      <c r="G15" s="29">
+        <v>2050</v>
+      </c>
+      <c r="H15" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" s="30">
+        <v>1061</v>
+      </c>
+      <c r="J15" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="K15" s="29" t="s">
+        <v>343</v>
+      </c>
+      <c r="L15" s="33">
+        <f t="shared" si="0"/>
+        <v>66567.14</v>
+      </c>
+      <c r="M15" s="36" t="s">
+        <v>508</v>
+      </c>
+      <c r="N15" s="29" t="s">
+        <v>509</v>
+      </c>
+      <c r="O15" s="33">
+        <f t="shared" si="1"/>
+        <v>25432.17</v>
+      </c>
+      <c r="P15" s="35">
+        <f t="shared" si="2"/>
+        <v>-41134.97</v>
+      </c>
+      <c r="Q15" s="29" t="s">
+        <v>344</v>
+      </c>
+      <c r="R15" s="29"/>
+      <c r="S15" s="32">
+        <f t="shared" si="3"/>
+        <v>-41156.19</v>
+      </c>
+      <c r="T15" s="29" t="s">
+        <v>345</v>
+      </c>
+      <c r="U15" s="31">
+        <v>45888</v>
+      </c>
+      <c r="V15" s="29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="6:22" ht="30">
+      <c r="F16" s="29">
+        <v>11</v>
+      </c>
+      <c r="G16" s="29">
+        <v>2060</v>
+      </c>
+      <c r="H16" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" s="30">
+        <v>5500</v>
+      </c>
+      <c r="J16" s="29" t="s">
+        <v>346</v>
+      </c>
+      <c r="K16" s="29" t="s">
+        <v>347</v>
+      </c>
+      <c r="L16" s="33">
+        <f t="shared" si="0"/>
+        <v>59730</v>
+      </c>
+      <c r="M16" s="36" t="s">
+        <v>450</v>
+      </c>
+      <c r="N16" s="29" t="s">
+        <v>510</v>
+      </c>
+      <c r="O16" s="33">
+        <f t="shared" si="1"/>
+        <v>59950</v>
+      </c>
+      <c r="P16" s="35">
+        <f t="shared" si="2"/>
+        <v>220</v>
+      </c>
+      <c r="Q16" s="29" t="s">
+        <v>348</v>
+      </c>
+      <c r="R16" s="29"/>
+      <c r="S16" s="32">
+        <f t="shared" si="3"/>
+        <v>495</v>
+      </c>
+      <c r="T16" s="29" t="s">
+        <v>349</v>
+      </c>
+      <c r="U16" s="31">
+        <v>45657</v>
+      </c>
+      <c r="V16" s="29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="6:22" ht="30">
+      <c r="F17" s="29">
+        <v>12</v>
+      </c>
+      <c r="G17" s="29">
+        <v>2070</v>
+      </c>
+      <c r="H17" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="I17" s="30">
+        <v>1500</v>
+      </c>
+      <c r="J17" s="29" t="s">
+        <v>350</v>
+      </c>
+      <c r="K17" s="29" t="s">
+        <v>351</v>
+      </c>
+      <c r="L17" s="33">
+        <f t="shared" si="0"/>
+        <v>47985</v>
+      </c>
+      <c r="M17" s="36" t="s">
+        <v>511</v>
+      </c>
+      <c r="N17" s="29" t="s">
+        <v>512</v>
+      </c>
+      <c r="O17" s="33">
+        <f t="shared" si="1"/>
+        <v>40935</v>
+      </c>
+      <c r="P17" s="35">
+        <f t="shared" si="2"/>
+        <v>-7050</v>
+      </c>
+      <c r="Q17" s="29" t="s">
+        <v>352</v>
+      </c>
+      <c r="R17" s="29"/>
+      <c r="S17" s="32">
+        <f t="shared" si="3"/>
+        <v>-7200</v>
+      </c>
+      <c r="T17" s="29" t="s">
+        <v>353</v>
+      </c>
+      <c r="U17" s="31">
+        <v>45657</v>
+      </c>
+      <c r="V17" s="29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="6:22" ht="30">
+      <c r="F18" s="29">
+        <v>13</v>
+      </c>
+      <c r="G18" s="29">
+        <v>2190</v>
+      </c>
+      <c r="H18" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="I18" s="30">
+        <v>1000</v>
+      </c>
+      <c r="J18" s="29" t="s">
+        <v>354</v>
+      </c>
+      <c r="K18" s="29" t="s">
+        <v>355</v>
+      </c>
+      <c r="L18" s="33">
+        <f t="shared" si="0"/>
+        <v>34500</v>
+      </c>
+      <c r="M18" s="36" t="s">
+        <v>356</v>
+      </c>
+      <c r="N18" s="29" t="s">
+        <v>357</v>
+      </c>
+      <c r="O18" s="33">
+        <f t="shared" si="1"/>
+        <v>21410</v>
+      </c>
+      <c r="P18" s="35">
+        <f t="shared" si="2"/>
+        <v>-13090</v>
+      </c>
+      <c r="Q18" s="29" t="s">
+        <v>358</v>
+      </c>
+      <c r="R18" s="29"/>
+      <c r="S18" s="32">
+        <f t="shared" si="3"/>
+        <v>-13090</v>
+      </c>
+      <c r="T18" s="29" t="s">
+        <v>359</v>
+      </c>
+      <c r="U18" s="31">
+        <v>45657</v>
+      </c>
+      <c r="V18" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="6:22" ht="30">
+      <c r="F19" s="29">
+        <v>14</v>
+      </c>
+      <c r="G19" s="29">
+        <v>2230</v>
+      </c>
+      <c r="H19" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="I19" s="30">
+        <v>1000</v>
+      </c>
+      <c r="J19" s="29" t="s">
+        <v>360</v>
+      </c>
+      <c r="K19" s="29" t="s">
+        <v>361</v>
+      </c>
+      <c r="L19" s="33">
+        <f t="shared" si="0"/>
+        <v>7620</v>
+      </c>
+      <c r="M19" s="36" t="s">
+        <v>362</v>
+      </c>
+      <c r="N19" s="29" t="s">
+        <v>363</v>
+      </c>
+      <c r="O19" s="33">
+        <f t="shared" si="1"/>
+        <v>15770</v>
+      </c>
+      <c r="P19" s="35">
+        <f t="shared" si="2"/>
+        <v>8150</v>
+      </c>
+      <c r="Q19" s="29" t="s">
+        <v>364</v>
+      </c>
+      <c r="R19" s="29"/>
+      <c r="S19" s="32">
+        <f t="shared" si="3"/>
+        <v>8150</v>
+      </c>
+      <c r="T19" s="29" t="s">
+        <v>365</v>
+      </c>
+      <c r="U19" s="31">
+        <v>45657</v>
+      </c>
+      <c r="V19" s="29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="6:22" ht="30">
+      <c r="F20" s="29">
+        <v>15</v>
+      </c>
+      <c r="G20" s="29">
+        <v>2280</v>
+      </c>
+      <c r="H20" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="I20" s="29">
+        <v>646</v>
+      </c>
+      <c r="J20" s="29" t="s">
+        <v>366</v>
+      </c>
+      <c r="K20" s="29" t="s">
+        <v>367</v>
+      </c>
+      <c r="L20" s="33">
+        <f t="shared" si="0"/>
+        <v>1292</v>
+      </c>
+      <c r="M20" s="36" t="s">
+        <v>513</v>
+      </c>
+      <c r="N20" s="29" t="s">
+        <v>514</v>
+      </c>
+      <c r="O20" s="33">
+        <f t="shared" si="1"/>
+        <v>29993.78</v>
+      </c>
+      <c r="P20" s="35">
+        <f t="shared" si="2"/>
+        <v>28701.78</v>
+      </c>
+      <c r="Q20" s="29" t="s">
+        <v>368</v>
+      </c>
+      <c r="R20" s="29"/>
+      <c r="S20" s="32">
+        <f t="shared" si="3"/>
+        <v>28740.54</v>
+      </c>
+      <c r="T20" s="29" t="s">
+        <v>369</v>
+      </c>
+      <c r="U20" s="31">
+        <v>45657</v>
+      </c>
+      <c r="V20" s="29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="6:22" ht="30">
+      <c r="F21" s="29">
+        <v>16</v>
+      </c>
+      <c r="G21" s="29">
+        <v>2290</v>
+      </c>
+      <c r="H21" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" s="30">
+        <v>3877</v>
+      </c>
+      <c r="J21" s="29" t="s">
+        <v>370</v>
+      </c>
+      <c r="K21" s="29" t="s">
+        <v>371</v>
+      </c>
+      <c r="L21" s="33">
+        <f t="shared" si="0"/>
+        <v>133136.18</v>
+      </c>
+      <c r="M21" s="36" t="s">
+        <v>372</v>
+      </c>
+      <c r="N21" s="29" t="s">
+        <v>373</v>
+      </c>
+      <c r="O21" s="33">
+        <f t="shared" si="1"/>
+        <v>134880.82999999999</v>
+      </c>
+      <c r="P21" s="35">
+        <f t="shared" si="2"/>
+        <v>1744.6499999999942</v>
+      </c>
+      <c r="Q21" s="29" t="s">
+        <v>374</v>
+      </c>
+      <c r="R21" s="29"/>
+      <c r="S21" s="32">
+        <f t="shared" si="3"/>
+        <v>1744.65</v>
+      </c>
+      <c r="T21" s="29" t="s">
+        <v>375</v>
+      </c>
+      <c r="U21" s="31">
+        <v>45657</v>
+      </c>
+      <c r="V21" s="29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="6:22" ht="30">
+      <c r="F22" s="29">
+        <v>17</v>
+      </c>
+      <c r="G22" s="36">
+        <v>2382</v>
+      </c>
+      <c r="H22" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="I22" s="37">
+        <v>1000</v>
+      </c>
+      <c r="J22" s="36" t="s">
+        <v>376</v>
+      </c>
+      <c r="K22" s="36" t="s">
+        <v>377</v>
+      </c>
+      <c r="L22" s="38">
+        <f t="shared" si="0"/>
+        <v>14720</v>
+      </c>
+      <c r="M22" s="36" t="s">
+        <v>515</v>
+      </c>
+      <c r="N22" s="36" t="s">
+        <v>516</v>
+      </c>
+      <c r="O22" s="38">
+        <f t="shared" si="1"/>
+        <v>14780</v>
+      </c>
+      <c r="P22" s="39">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="Q22" s="36" t="s">
+        <v>378</v>
+      </c>
+      <c r="R22" s="29"/>
+      <c r="S22" s="32">
+        <f t="shared" si="3"/>
+        <v>140</v>
+      </c>
+      <c r="T22" s="29" t="s">
+        <v>379</v>
+      </c>
+      <c r="U22" s="31">
+        <v>45657</v>
+      </c>
+      <c r="V22" s="29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="6:22" ht="30">
+      <c r="F23" s="29">
+        <v>18</v>
+      </c>
+      <c r="G23" s="29">
+        <v>3040</v>
+      </c>
+      <c r="H23" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" s="29">
+        <v>972</v>
+      </c>
+      <c r="J23" s="29" t="s">
+        <v>380</v>
+      </c>
+      <c r="K23" s="29" t="s">
+        <v>381</v>
+      </c>
+      <c r="L23" s="33">
+        <f t="shared" si="0"/>
+        <v>60759.72</v>
+      </c>
+      <c r="M23" s="36" t="s">
+        <v>382</v>
+      </c>
+      <c r="N23" s="29" t="s">
+        <v>383</v>
+      </c>
+      <c r="O23" s="33">
+        <f t="shared" si="1"/>
+        <v>37101.24</v>
+      </c>
+      <c r="P23" s="35">
+        <f t="shared" si="2"/>
+        <v>-23658.480000000003</v>
+      </c>
+      <c r="Q23" s="29" t="s">
+        <v>384</v>
+      </c>
+      <c r="R23" s="29"/>
+      <c r="S23" s="32">
+        <f t="shared" si="3"/>
+        <v>-23658.48</v>
+      </c>
+      <c r="T23" s="29" t="s">
+        <v>385</v>
+      </c>
+      <c r="U23" s="31">
+        <v>45657</v>
+      </c>
+      <c r="V23" s="29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="6:22" ht="30">
+      <c r="F24" s="29">
+        <v>19</v>
+      </c>
+      <c r="G24" s="29">
+        <v>4001</v>
+      </c>
+      <c r="H24" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="I24" s="30">
+        <v>9500</v>
+      </c>
+      <c r="J24" s="29" t="s">
+        <v>386</v>
+      </c>
+      <c r="K24" s="29" t="s">
+        <v>387</v>
+      </c>
+      <c r="L24" s="33">
+        <f t="shared" si="0"/>
+        <v>102125</v>
+      </c>
+      <c r="M24" s="36" t="s">
+        <v>517</v>
+      </c>
+      <c r="N24" s="29" t="s">
+        <v>518</v>
+      </c>
+      <c r="O24" s="33">
+        <f t="shared" si="1"/>
+        <v>74670</v>
+      </c>
+      <c r="P24" s="35">
+        <f t="shared" si="2"/>
+        <v>-27455</v>
+      </c>
+      <c r="Q24" s="29" t="s">
+        <v>388</v>
+      </c>
+      <c r="R24" s="29"/>
+      <c r="S24" s="32">
+        <f t="shared" si="3"/>
+        <v>199120</v>
+      </c>
+      <c r="T24" s="29" t="s">
+        <v>389</v>
+      </c>
+      <c r="U24" s="31">
+        <v>45657</v>
+      </c>
+      <c r="V24" s="29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="6:22" ht="30">
+      <c r="F25" s="29">
+        <v>20</v>
+      </c>
+      <c r="G25" s="29">
+        <v>4084</v>
+      </c>
+      <c r="H25" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="I25" s="29">
+        <v>10</v>
+      </c>
+      <c r="J25" s="29" t="s">
+        <v>390</v>
+      </c>
+      <c r="K25" s="29" t="s">
+        <v>391</v>
+      </c>
+      <c r="L25" s="33">
+        <f t="shared" si="0"/>
+        <v>259.2</v>
+      </c>
+      <c r="M25" s="36" t="s">
+        <v>392</v>
+      </c>
+      <c r="N25" s="29" t="s">
+        <v>393</v>
+      </c>
+      <c r="O25" s="33">
+        <f t="shared" si="1"/>
+        <v>289</v>
+      </c>
+      <c r="P25" s="35">
+        <f t="shared" si="2"/>
+        <v>29.800000000000011</v>
+      </c>
+      <c r="Q25" s="29" t="s">
+        <v>394</v>
+      </c>
+      <c r="R25" s="29"/>
+      <c r="S25" s="32">
+        <f t="shared" si="3"/>
+        <v>29.8</v>
+      </c>
+      <c r="T25" s="29" t="s">
+        <v>395</v>
+      </c>
+      <c r="U25" s="31">
+        <v>45657</v>
+      </c>
+      <c r="V25" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="6:22" ht="30">
+      <c r="F26" s="29">
+        <v>21</v>
+      </c>
+      <c r="G26" s="29">
+        <v>4110</v>
+      </c>
+      <c r="H26" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="I26" s="30">
+        <v>6800</v>
+      </c>
+      <c r="J26" s="29" t="s">
+        <v>396</v>
+      </c>
+      <c r="K26" s="29" t="s">
+        <v>397</v>
+      </c>
+      <c r="L26" s="33">
+        <f t="shared" si="0"/>
+        <v>15368</v>
+      </c>
+      <c r="M26" s="36" t="s">
+        <v>519</v>
+      </c>
+      <c r="N26" s="29" t="s">
+        <v>520</v>
+      </c>
+      <c r="O26" s="33">
+        <f t="shared" si="1"/>
+        <v>15776</v>
+      </c>
+      <c r="P26" s="35">
+        <f t="shared" si="2"/>
+        <v>408</v>
+      </c>
+      <c r="Q26" s="29" t="s">
+        <v>398</v>
+      </c>
+      <c r="R26" s="29"/>
+      <c r="S26" s="32">
+        <f t="shared" si="3"/>
+        <v>151504</v>
+      </c>
+      <c r="T26" s="29" t="s">
+        <v>399</v>
+      </c>
+      <c r="U26" s="31">
+        <v>45657</v>
+      </c>
+      <c r="V26" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="6:22" ht="30">
+      <c r="F27" s="29">
+        <v>22</v>
+      </c>
+      <c r="G27" s="29">
+        <v>4161</v>
+      </c>
+      <c r="H27" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="I27" s="30">
+        <v>4000</v>
+      </c>
+      <c r="J27" s="29" t="s">
+        <v>400</v>
+      </c>
+      <c r="K27" s="29" t="s">
+        <v>401</v>
+      </c>
+      <c r="L27" s="33">
+        <f t="shared" si="0"/>
+        <v>31160</v>
+      </c>
+      <c r="M27" s="36" t="s">
+        <v>521</v>
+      </c>
+      <c r="N27" s="29" t="s">
+        <v>522</v>
+      </c>
+      <c r="O27" s="33">
+        <f t="shared" si="1"/>
+        <v>22640</v>
+      </c>
+      <c r="P27" s="35">
+        <f t="shared" si="2"/>
+        <v>-8520</v>
+      </c>
+      <c r="Q27" s="29" t="s">
+        <v>402</v>
+      </c>
+      <c r="R27" s="29"/>
+      <c r="S27" s="32">
+        <f t="shared" si="3"/>
+        <v>102680</v>
+      </c>
+      <c r="T27" s="29" t="s">
+        <v>403</v>
+      </c>
+      <c r="U27" s="31">
+        <v>45657</v>
+      </c>
+      <c r="V27" s="29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="6:22" ht="30">
+      <c r="F28" s="29">
+        <v>23</v>
+      </c>
+      <c r="G28" s="29">
+        <v>4190</v>
+      </c>
+      <c r="H28" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="I28" s="30">
+        <v>8573</v>
+      </c>
+      <c r="J28" s="29" t="s">
+        <v>404</v>
+      </c>
+      <c r="K28" s="29" t="s">
+        <v>405</v>
+      </c>
+      <c r="L28" s="33">
+        <f t="shared" si="0"/>
+        <v>116335.61</v>
+      </c>
+      <c r="M28" s="36" t="s">
+        <v>406</v>
+      </c>
+      <c r="N28" s="29" t="s">
+        <v>407</v>
+      </c>
+      <c r="O28" s="33">
+        <f t="shared" si="1"/>
+        <v>217239.82</v>
+      </c>
+      <c r="P28" s="35">
+        <f t="shared" si="2"/>
+        <v>100904.21</v>
+      </c>
+      <c r="Q28" s="29" t="s">
+        <v>408</v>
+      </c>
+      <c r="R28" s="29"/>
+      <c r="S28" s="32">
+        <f t="shared" si="3"/>
+        <v>100904.21</v>
+      </c>
+      <c r="T28" s="29" t="s">
+        <v>409</v>
+      </c>
+      <c r="U28" s="31">
+        <v>45657</v>
+      </c>
+      <c r="V28" s="29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="6:22" ht="30">
+      <c r="F29" s="29">
+        <v>24</v>
+      </c>
+      <c r="G29" s="29">
+        <v>4322</v>
+      </c>
+      <c r="H29" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="I29" s="30">
+        <v>4000</v>
+      </c>
+      <c r="J29" s="29" t="s">
+        <v>410</v>
+      </c>
+      <c r="K29" s="29" t="s">
+        <v>411</v>
+      </c>
+      <c r="L29" s="33">
+        <f t="shared" si="0"/>
+        <v>57720</v>
+      </c>
+      <c r="M29" s="36" t="s">
+        <v>412</v>
+      </c>
+      <c r="N29" s="29" t="s">
+        <v>413</v>
+      </c>
+      <c r="O29" s="33">
+        <f t="shared" si="1"/>
+        <v>114560</v>
+      </c>
+      <c r="P29" s="35">
+        <f t="shared" si="2"/>
+        <v>56840</v>
+      </c>
+      <c r="Q29" s="29" t="s">
+        <v>414</v>
+      </c>
+      <c r="R29" s="29"/>
+      <c r="S29" s="32">
+        <f t="shared" si="3"/>
+        <v>56840</v>
+      </c>
+      <c r="T29" s="29" t="s">
+        <v>415</v>
+      </c>
+      <c r="U29" s="31">
+        <v>45657</v>
+      </c>
+      <c r="V29" s="29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="6:22" ht="30">
+      <c r="F30" s="29">
+        <v>25</v>
+      </c>
+      <c r="G30" s="29">
+        <v>4323</v>
+      </c>
+      <c r="H30" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="I30" s="30">
+        <v>1300</v>
+      </c>
+      <c r="J30" s="29" t="s">
+        <v>416</v>
+      </c>
+      <c r="K30" s="29" t="s">
+        <v>417</v>
+      </c>
+      <c r="L30" s="33">
+        <f t="shared" si="0"/>
+        <v>55718</v>
+      </c>
+      <c r="M30" s="36" t="s">
+        <v>418</v>
+      </c>
+      <c r="N30" s="29" t="s">
+        <v>419</v>
+      </c>
+      <c r="O30" s="33">
+        <f t="shared" si="1"/>
+        <v>50973</v>
+      </c>
+      <c r="P30" s="35">
+        <f t="shared" si="2"/>
+        <v>-4745</v>
+      </c>
+      <c r="Q30" s="29" t="s">
+        <v>420</v>
+      </c>
+      <c r="R30" s="29"/>
+      <c r="S30" s="32">
+        <f t="shared" si="3"/>
+        <v>-4745</v>
+      </c>
+      <c r="T30" s="29" t="s">
+        <v>421</v>
+      </c>
+      <c r="U30" s="31">
+        <v>45657</v>
+      </c>
+      <c r="V30" s="29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="6:22" ht="30">
+      <c r="F31" s="29">
+        <v>26</v>
+      </c>
+      <c r="G31" s="29">
+        <v>4325</v>
+      </c>
+      <c r="H31" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="I31" s="30">
+        <v>1015</v>
+      </c>
+      <c r="J31" s="29" t="s">
+        <v>422</v>
+      </c>
+      <c r="K31" s="29" t="s">
+        <v>423</v>
+      </c>
+      <c r="L31" s="33">
+        <f t="shared" si="0"/>
+        <v>23690.1</v>
+      </c>
+      <c r="M31" s="36" t="s">
+        <v>424</v>
+      </c>
+      <c r="N31" s="29" t="s">
+        <v>425</v>
+      </c>
+      <c r="O31" s="33">
+        <f t="shared" si="1"/>
+        <v>30409.4</v>
+      </c>
+      <c r="P31" s="35">
+        <f t="shared" si="2"/>
+        <v>6719.3000000000029</v>
+      </c>
+      <c r="Q31" s="29" t="s">
+        <v>426</v>
+      </c>
+      <c r="R31" s="29"/>
+      <c r="S31" s="32">
+        <f t="shared" si="3"/>
+        <v>6719.3</v>
+      </c>
+      <c r="T31" s="29" t="s">
+        <v>427</v>
+      </c>
+      <c r="U31" s="31">
+        <v>45657</v>
+      </c>
+      <c r="V31" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="6:22" ht="30">
+      <c r="F32" s="29">
+        <v>27</v>
+      </c>
+      <c r="G32" s="29">
+        <v>4338</v>
+      </c>
+      <c r="H32" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="I32" s="30">
+        <v>3000</v>
+      </c>
+      <c r="J32" s="29" t="s">
+        <v>428</v>
+      </c>
+      <c r="K32" s="29" t="s">
+        <v>429</v>
+      </c>
+      <c r="L32" s="33">
+        <f t="shared" si="0"/>
+        <v>24330</v>
+      </c>
+      <c r="M32" s="36" t="s">
+        <v>430</v>
+      </c>
+      <c r="N32" s="29" t="s">
+        <v>431</v>
+      </c>
+      <c r="O32" s="33">
+        <f t="shared" si="1"/>
+        <v>115380</v>
+      </c>
+      <c r="P32" s="35">
+        <f t="shared" si="2"/>
+        <v>91050</v>
+      </c>
+      <c r="Q32" s="29" t="s">
+        <v>432</v>
+      </c>
+      <c r="R32" s="29"/>
+      <c r="S32" s="32">
+        <f t="shared" si="3"/>
+        <v>91050</v>
+      </c>
+      <c r="T32" s="29" t="s">
+        <v>433</v>
+      </c>
+      <c r="U32" s="31">
+        <v>45657</v>
+      </c>
+      <c r="V32" s="29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="6:22" ht="30">
+      <c r="F33" s="29">
+        <v>28</v>
+      </c>
+      <c r="G33" s="29">
+        <v>5110</v>
+      </c>
+      <c r="H33" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="I33" s="30">
+        <v>3000</v>
+      </c>
+      <c r="J33" s="29" t="s">
+        <v>434</v>
+      </c>
+      <c r="K33" s="29" t="s">
+        <v>435</v>
+      </c>
+      <c r="L33" s="33">
+        <f t="shared" si="0"/>
+        <v>51150</v>
+      </c>
+      <c r="M33" s="36" t="s">
+        <v>436</v>
+      </c>
+      <c r="N33" s="29" t="s">
+        <v>437</v>
+      </c>
+      <c r="O33" s="33">
+        <f t="shared" si="1"/>
+        <v>83760</v>
+      </c>
+      <c r="P33" s="35">
+        <f t="shared" si="2"/>
+        <v>32610</v>
+      </c>
+      <c r="Q33" s="29" t="s">
+        <v>438</v>
+      </c>
+      <c r="R33" s="29"/>
+      <c r="S33" s="32">
+        <f t="shared" si="3"/>
+        <v>32610</v>
+      </c>
+      <c r="T33" s="29" t="s">
+        <v>439</v>
+      </c>
+      <c r="U33" s="31">
+        <v>45657</v>
+      </c>
+      <c r="V33" s="29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="6:22" ht="30">
+      <c r="F34" s="29">
+        <v>29</v>
+      </c>
+      <c r="G34" s="29">
+        <v>6010</v>
+      </c>
+      <c r="H34" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="I34" s="30">
+        <v>2967</v>
+      </c>
+      <c r="J34" s="29" t="s">
+        <v>440</v>
+      </c>
+      <c r="K34" s="29" t="s">
+        <v>441</v>
+      </c>
+      <c r="L34" s="33">
+        <f t="shared" si="0"/>
+        <v>66104.759999999995</v>
+      </c>
+      <c r="M34" s="36" t="s">
+        <v>442</v>
+      </c>
+      <c r="N34" s="29" t="s">
+        <v>443</v>
+      </c>
+      <c r="O34" s="33">
+        <f t="shared" si="1"/>
+        <v>100343.94</v>
+      </c>
+      <c r="P34" s="35">
+        <f t="shared" si="2"/>
+        <v>34239.180000000008</v>
+      </c>
+      <c r="Q34" s="29" t="s">
+        <v>444</v>
+      </c>
+      <c r="R34" s="29"/>
+      <c r="S34" s="32">
+        <f t="shared" si="3"/>
+        <v>34239.18</v>
+      </c>
+      <c r="T34" s="29" t="s">
+        <v>445</v>
+      </c>
+      <c r="U34" s="31">
+        <v>45657</v>
+      </c>
+      <c r="V34" s="29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="6:22" ht="30">
+      <c r="F35" s="29">
+        <v>30</v>
+      </c>
+      <c r="G35" s="29">
+        <v>7010</v>
+      </c>
+      <c r="H35" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="I35" s="30">
+        <v>3000</v>
+      </c>
+      <c r="J35" s="29" t="s">
+        <v>446</v>
+      </c>
+      <c r="K35" s="29" t="s">
+        <v>447</v>
+      </c>
+      <c r="L35" s="33">
+        <f t="shared" si="0"/>
+        <v>126660</v>
+      </c>
+      <c r="M35" s="36" t="s">
+        <v>523</v>
+      </c>
+      <c r="N35" s="29" t="s">
+        <v>524</v>
+      </c>
+      <c r="O35" s="33">
+        <f t="shared" si="1"/>
+        <v>127500</v>
+      </c>
+      <c r="P35" s="35">
+        <f t="shared" si="2"/>
+        <v>840</v>
+      </c>
+      <c r="Q35" s="29" t="s">
+        <v>448</v>
+      </c>
+      <c r="R35" s="29"/>
+      <c r="S35" s="32">
+        <f t="shared" si="3"/>
+        <v>720</v>
+      </c>
+      <c r="T35" s="29" t="s">
+        <v>449</v>
+      </c>
+      <c r="U35" s="31">
+        <v>45657</v>
+      </c>
+      <c r="V35" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="6:22" ht="30">
+      <c r="F36" s="29">
+        <v>31</v>
+      </c>
+      <c r="G36" s="29">
+        <v>7030</v>
+      </c>
+      <c r="H36" s="29" t="s">
+        <v>257</v>
+      </c>
+      <c r="I36" s="30">
+        <v>9400</v>
+      </c>
+      <c r="J36" s="29" t="s">
+        <v>450</v>
+      </c>
+      <c r="K36" s="29" t="s">
+        <v>451</v>
+      </c>
+      <c r="L36" s="33">
+        <f t="shared" si="0"/>
+        <v>102460</v>
+      </c>
+      <c r="M36" s="36" t="s">
+        <v>525</v>
+      </c>
+      <c r="N36" s="29" t="s">
+        <v>526</v>
+      </c>
+      <c r="O36" s="33">
+        <f t="shared" si="1"/>
+        <v>102366</v>
+      </c>
+      <c r="P36" s="35">
+        <f t="shared" si="2"/>
+        <v>-94</v>
+      </c>
+      <c r="Q36" s="29" t="s">
+        <v>452</v>
+      </c>
+      <c r="R36" s="29"/>
+      <c r="S36" s="32">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T36" s="29" t="s">
+        <v>453</v>
+      </c>
+      <c r="U36" s="31">
+        <v>45657</v>
+      </c>
+      <c r="V36" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="6:22" ht="30">
+      <c r="F37" s="29">
+        <v>32</v>
+      </c>
+      <c r="G37" s="29">
+        <v>8150</v>
+      </c>
+      <c r="H37" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="I37" s="30">
+        <v>1500</v>
+      </c>
+      <c r="J37" s="29" t="s">
+        <v>454</v>
+      </c>
+      <c r="K37" s="29" t="s">
+        <v>455</v>
+      </c>
+      <c r="L37" s="33">
+        <f t="shared" si="0"/>
+        <v>22710</v>
+      </c>
+      <c r="M37" s="36" t="s">
+        <v>356</v>
+      </c>
+      <c r="N37" s="29" t="s">
+        <v>456</v>
+      </c>
+      <c r="O37" s="33">
+        <f t="shared" si="1"/>
+        <v>32115</v>
+      </c>
+      <c r="P37" s="35">
+        <f t="shared" si="2"/>
+        <v>9405</v>
+      </c>
+      <c r="Q37" s="29" t="s">
+        <v>457</v>
+      </c>
+      <c r="R37" s="29"/>
+      <c r="S37" s="32">
+        <f t="shared" si="3"/>
+        <v>9405</v>
+      </c>
+      <c r="T37" s="29" t="s">
+        <v>458</v>
+      </c>
+      <c r="U37" s="31">
+        <v>45657</v>
+      </c>
+      <c r="V37" s="29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="6:22" ht="30">
+      <c r="F38" s="29">
+        <v>33</v>
+      </c>
+      <c r="G38" s="29">
+        <v>9408</v>
+      </c>
+      <c r="H38" s="29" t="s">
+        <v>459</v>
+      </c>
+      <c r="I38" s="30">
+        <v>1000</v>
+      </c>
+      <c r="J38" s="29" t="s">
+        <v>460</v>
+      </c>
+      <c r="K38" s="29" t="s">
+        <v>461</v>
+      </c>
+      <c r="L38" s="33">
+        <f t="shared" si="0"/>
+        <v>11190</v>
+      </c>
+      <c r="M38" s="36" t="s">
+        <v>462</v>
+      </c>
+      <c r="N38" s="29" t="s">
+        <v>463</v>
+      </c>
+      <c r="O38" s="33">
+        <f t="shared" si="1"/>
+        <v>24550</v>
+      </c>
+      <c r="P38" s="35">
+        <f t="shared" si="2"/>
+        <v>13360</v>
+      </c>
+      <c r="Q38" s="29" t="s">
+        <v>464</v>
+      </c>
+      <c r="R38" s="29"/>
+      <c r="S38" s="32">
+        <f t="shared" si="3"/>
+        <v>13360</v>
+      </c>
+      <c r="T38" s="29" t="s">
+        <v>465</v>
+      </c>
+      <c r="U38" s="31">
+        <v>45657</v>
+      </c>
+      <c r="V38" s="29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="6:22" ht="30">
+      <c r="F39" s="29">
+        <v>34</v>
+      </c>
+      <c r="G39" s="29">
+        <v>1303</v>
+      </c>
+      <c r="H39" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="I39" s="30">
+        <v>9750</v>
+      </c>
+      <c r="J39" s="29" t="s">
+        <v>466</v>
+      </c>
+      <c r="K39" s="29" t="s">
+        <v>467</v>
+      </c>
+      <c r="L39" s="33">
+        <f t="shared" si="0"/>
+        <v>82867.5</v>
+      </c>
+      <c r="M39" s="36" t="s">
+        <v>468</v>
+      </c>
+      <c r="N39" s="29" t="s">
+        <v>469</v>
+      </c>
+      <c r="O39" s="33">
+        <f t="shared" si="1"/>
+        <v>379762.5</v>
+      </c>
+      <c r="P39" s="35">
+        <f t="shared" si="2"/>
+        <v>296895</v>
+      </c>
+      <c r="Q39" s="29" t="s">
+        <v>470</v>
+      </c>
+      <c r="R39" s="29"/>
+      <c r="S39" s="32">
+        <f t="shared" si="3"/>
+        <v>296895</v>
+      </c>
+      <c r="T39" s="29" t="s">
+        <v>471</v>
+      </c>
+      <c r="U39" s="31">
+        <v>45657</v>
+      </c>
+      <c r="V39" s="29" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="40" spans="6:22" ht="30">
+      <c r="F40" s="29">
+        <v>35</v>
+      </c>
+      <c r="G40" s="29">
+        <v>4007</v>
+      </c>
+      <c r="H40" s="29" t="s">
+        <v>194</v>
+      </c>
+      <c r="I40" s="30">
+        <v>1000</v>
+      </c>
+      <c r="J40" s="29" t="s">
+        <v>473</v>
+      </c>
+      <c r="K40" s="29" t="s">
+        <v>474</v>
+      </c>
+      <c r="L40" s="33">
+        <f t="shared" si="0"/>
+        <v>38890</v>
+      </c>
+      <c r="M40" s="36" t="s">
+        <v>475</v>
+      </c>
+      <c r="N40" s="29" t="s">
+        <v>476</v>
+      </c>
+      <c r="O40" s="33">
+        <f t="shared" si="1"/>
+        <v>18840</v>
+      </c>
+      <c r="P40" s="35">
+        <f t="shared" si="2"/>
+        <v>-20050</v>
+      </c>
+      <c r="Q40" s="29" t="s">
+        <v>477</v>
+      </c>
+      <c r="R40" s="29"/>
+      <c r="S40" s="32">
+        <f t="shared" si="3"/>
+        <v>-20050</v>
+      </c>
+      <c r="T40" s="29" t="s">
+        <v>478</v>
+      </c>
+      <c r="U40" s="31">
+        <v>45657</v>
+      </c>
+      <c r="V40" s="29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="6:22" ht="30">
+      <c r="F41" s="29">
+        <v>36</v>
+      </c>
+      <c r="G41" s="29">
+        <v>4130</v>
+      </c>
+      <c r="H41" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="I41" s="30">
+        <v>8470</v>
+      </c>
+      <c r="J41" s="29" t="s">
+        <v>479</v>
+      </c>
+      <c r="K41" s="29" t="s">
+        <v>480</v>
+      </c>
+      <c r="L41" s="33">
+        <f t="shared" si="0"/>
+        <v>39893.699999999997</v>
+      </c>
+      <c r="M41" s="36" t="s">
+        <v>481</v>
+      </c>
+      <c r="N41" s="29" t="s">
+        <v>482</v>
+      </c>
+      <c r="O41" s="33">
+        <f t="shared" si="1"/>
+        <v>205651.6</v>
+      </c>
+      <c r="P41" s="35">
+        <f t="shared" si="2"/>
+        <v>165757.90000000002</v>
+      </c>
+      <c r="Q41" s="29" t="s">
+        <v>483</v>
+      </c>
+      <c r="R41" s="29"/>
+      <c r="S41" s="32">
+        <f t="shared" si="3"/>
+        <v>165757.9</v>
+      </c>
+      <c r="T41" s="29" t="s">
+        <v>484</v>
+      </c>
+      <c r="U41" s="31">
+        <v>45657</v>
+      </c>
+      <c r="V41" s="29" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="42" spans="6:22" ht="30">
+      <c r="F42" s="29">
+        <v>37</v>
+      </c>
+      <c r="G42" s="29">
+        <v>2222</v>
+      </c>
+      <c r="H42" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="I42" s="30">
+        <v>2781</v>
+      </c>
+      <c r="J42" s="29" t="s">
+        <v>486</v>
+      </c>
+      <c r="K42" s="29" t="s">
+        <v>487</v>
+      </c>
+      <c r="L42" s="33">
+        <f t="shared" si="0"/>
+        <v>74150.25</v>
+      </c>
+      <c r="M42" s="36" t="s">
+        <v>488</v>
+      </c>
+      <c r="N42" s="29" t="s">
+        <v>489</v>
+      </c>
+      <c r="O42" s="33">
+        <f t="shared" si="1"/>
+        <v>87545.88</v>
+      </c>
+      <c r="P42" s="35">
+        <f t="shared" si="2"/>
+        <v>13395.630000000005</v>
+      </c>
+      <c r="Q42" s="29" t="s">
+        <v>490</v>
+      </c>
+      <c r="R42" s="29"/>
+      <c r="S42" s="32">
+        <f t="shared" si="3"/>
+        <v>13395.63</v>
+      </c>
+      <c r="T42" s="29" t="s">
+        <v>491</v>
+      </c>
+      <c r="U42" s="31">
+        <v>45657</v>
+      </c>
+      <c r="V42" s="29" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="43" spans="6:22">
+      <c r="L43" s="34">
+        <f>SUM(L6:L42)</f>
+        <v>2316197.88</v>
+      </c>
+      <c r="O43" s="34">
+        <f>SUM(O6:O42)</f>
+        <v>2982236.23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{668E8E06-E601-4F27-B9CE-2FA802A83F33}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="D4:Y268"/>
@@ -7963,16 +10801,16 @@
       <selection activeCell="J10" sqref="J10:M268"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="8" max="11" width="9" style="18"/>
-    <col min="12" max="12" width="24.125" style="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="40.875" style="18" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.140625" style="24" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="40.85546875" style="18" bestFit="1" customWidth="1"/>
     <col min="17" max="21" width="9" customWidth="1"/>
-    <col min="22" max="22" width="33.5" customWidth="1"/>
+    <col min="22" max="22" width="33.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="5:25" ht="15" thickBot="1"/>
+    <row r="4" spans="5:25" ht="15.75" thickBot="1"/>
     <row r="5" spans="5:25" ht="18">
       <c r="U5" s="9"/>
       <c r="V5" s="10"/>
@@ -8236,7 +11074,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="17" spans="5:25">
+    <row r="17" spans="5:25" ht="27">
       <c r="E17" s="16" t="s">
         <v>52</v>
       </c>
@@ -11194,7 +14032,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="120" spans="4:25">
+    <row r="120" spans="4:25" ht="27">
       <c r="H120" s="19">
         <v>111</v>
       </c>
@@ -11223,7 +14061,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="121" spans="4:25">
+    <row r="121" spans="4:25" ht="27">
       <c r="H121" s="20">
         <v>112</v>
       </c>
@@ -11242,7 +14080,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="122" spans="4:25">
+    <row r="122" spans="4:25" ht="27">
       <c r="H122" s="19">
         <v>113</v>
       </c>
@@ -11271,7 +14109,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="123" spans="4:25">
+    <row r="123" spans="4:25" ht="27">
       <c r="H123" s="19">
         <v>114</v>
       </c>
@@ -11300,7 +14138,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="124" spans="4:25">
+    <row r="124" spans="4:25" ht="27">
       <c r="H124" s="20">
         <v>115</v>
       </c>
@@ -11329,7 +14167,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="125" spans="4:25">
+    <row r="125" spans="4:25" ht="27">
       <c r="H125" s="19">
         <v>116</v>
       </c>
@@ -11358,7 +14196,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="126" spans="4:25">
+    <row r="126" spans="4:25" ht="27">
       <c r="H126" s="19">
         <v>117</v>
       </c>
@@ -11387,7 +14225,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="127" spans="4:25">
+    <row r="127" spans="4:25" ht="27">
       <c r="H127" s="20">
         <v>118</v>
       </c>
@@ -14546,7 +17384,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="237" spans="6:25">
+    <row r="237" spans="6:25" ht="30">
       <c r="H237" s="19">
         <v>228</v>
       </c>
@@ -14971,7 +17809,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="252" spans="6:25">
+    <row r="252" spans="6:25" ht="30">
       <c r="H252" s="20">
         <v>243</v>
       </c>
@@ -15577,14 +18415,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
@@ -15592,7 +18430,7 @@
     <col min="5" max="5" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -15614,13 +18452,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{262432D4-593E-4ECC-A6E0-86D849179F27}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>